<commit_message>
feat(widget): add common properties
</commit_message>
<xml_diff>
--- a/docs/课程安排.xlsx
+++ b/docs/课程安排.xlsx
@@ -1505,10 +1505,10 @@
   <sheetPr/>
   <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I57" sqref="I57"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1516,8 +1516,13 @@
     <col min="1" max="1" width="5.25" customWidth="1"/>
     <col min="2" max="2" width="6.40625" customWidth="1"/>
     <col min="3" max="3" width="4.25" customWidth="1"/>
-    <col min="4" max="9" width="20.1796875" customWidth="1"/>
-    <col min="10" max="10" width="27.859375" customWidth="1"/>
+    <col min="4" max="4" width="5" customWidth="1"/>
+    <col min="5" max="5" width="57.8125" customWidth="1"/>
+    <col min="6" max="6" width="5.125" customWidth="1"/>
+    <col min="7" max="7" width="4.5" customWidth="1"/>
+    <col min="8" max="8" width="57.8125" customWidth="1"/>
+    <col min="9" max="9" width="4.125" customWidth="1"/>
+    <col min="10" max="10" width="30.125" customWidth="1"/>
     <col min="11" max="11" width="4.5546875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>